<commit_message>
feat: first impl to save data to database
</commit_message>
<xml_diff>
--- a/db/AssortimentGPK.xlsx
+++ b/db/AssortimentGPK.xlsx
@@ -10,14 +10,14 @@
     <sheet name="ASSORTIMENTGPK" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ASSORTIMENTGPK!$A$1:$F$3876</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ASSORTIMENTGPK!$A$1:$F$3878</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19381" uniqueCount="9937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19390" uniqueCount="9941">
   <si>
     <t>GPKODE</t>
   </si>
@@ -29828,6 +29828,18 @@
   </si>
   <si>
     <t>LINEZOLID 2MG/ML INFVLST</t>
+  </si>
+  <si>
+    <t>NATRIUMCHLORIDE 3% INFVLST ZAK 100ML</t>
+  </si>
+  <si>
+    <t>NATRIUMCHLORIDE 3% 100ML</t>
+  </si>
+  <si>
+    <t>MAGNESIUMSULFAAT 100MG/ML ( 0,4MMOL/ML) INJVLST AMPUL 10ML</t>
+  </si>
+  <si>
+    <t>MAGNESIUMSULFAAT INJVLST 100MG/ML</t>
   </si>
 </sst>
 </file>
@@ -30164,10 +30176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3876"/>
+  <dimension ref="A1:F3878"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3307" sqref="C3307"/>
+    <sheetView tabSelected="1" topLeftCell="A3837" workbookViewId="0">
+      <selection activeCell="A3878" sqref="A3878"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -107698,8 +107710,48 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3877" spans="1:6">
+      <c r="A3877" s="1">
+        <v>147419</v>
+      </c>
+      <c r="B3877" t="s">
+        <v>9937</v>
+      </c>
+      <c r="C3877" t="s">
+        <v>9937</v>
+      </c>
+      <c r="D3877" t="s">
+        <v>9938</v>
+      </c>
+      <c r="E3877" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F3877" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3878" spans="1:6">
+      <c r="A3878">
+        <v>14058413</v>
+      </c>
+      <c r="B3878" t="s">
+        <v>9939</v>
+      </c>
+      <c r="C3878" t="s">
+        <v>9940</v>
+      </c>
+      <c r="D3878" t="s">
+        <v>5481</v>
+      </c>
+      <c r="E3878" t="s">
+        <v>5470</v>
+      </c>
+      <c r="F3878">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F3876"/>
+  <autoFilter ref="A1:F3878"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: improved cont med input
</commit_message>
<xml_diff>
--- a/db/AssortimentGPK.xlsx
+++ b/db/AssortimentGPK.xlsx
@@ -30178,8 +30178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3878"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3837" workbookViewId="0">
-      <selection activeCell="A3878" sqref="A3878"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1953" sqref="C1953"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>